<commit_message>
deleted useless csv files, updated variable_simulator function to fix some bugs
</commit_message>
<xml_diff>
--- a/IdealGasLawPressure.xlsx
+++ b/IdealGasLawPressure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xaos\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xaos\Desktop\General Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3647F042-E3FC-4E5B-B380-B45BA0E853D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6261C36A-4D47-4D81-8DB7-587C1FA29F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Pressure per unit Area (p)</t>
+    <t>Pressure_per_unit_Area_p</t>
   </si>
   <si>
-    <t>Weight on Piston (N)</t>
+    <t>Weight_on_Piston_N</t>
   </si>
 </sst>
 </file>
@@ -350,11 +350,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>